<commit_message>
Renombrar casos en excel
</commit_message>
<xml_diff>
--- a/TP1/2daEntrega/LoteDePruebas/ResultadoPruebas.xlsx
+++ b/TP1/2daEntrega/LoteDePruebas/ResultadoPruebas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -43,11 +43,89 @@
           <t xml:space="preserve">
 SALIDA:
 SI
+2 2 3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+SALIDA:
+NO</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+SALIDA:
+SI 2
+3 2
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+SALIDA:
+SI
 2 6 8</t>
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="0">
+    <comment ref="J4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -71,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="0">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -95,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0">
+    <comment ref="E6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -120,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0">
+    <comment ref="F6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -146,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0">
+    <comment ref="J6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -171,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0">
+    <comment ref="C7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -196,7 +274,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0">
+    <comment ref="E7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -221,7 +299,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0">
+    <comment ref="F7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -247,7 +325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="0">
+    <comment ref="J7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -272,7 +350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0">
+    <comment ref="E8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -298,7 +376,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="0">
+    <comment ref="F8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -324,7 +402,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H7" authorId="0">
+    <comment ref="H8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -350,7 +428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J7" authorId="0">
+    <comment ref="J8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -374,7 +452,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0">
+    <comment ref="B9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -400,7 +478,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0">
+    <comment ref="C9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -426,7 +504,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0">
+    <comment ref="D9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -452,7 +530,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0">
+    <comment ref="E9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -478,7 +556,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0">
+    <comment ref="F9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -504,7 +582,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0">
+    <comment ref="G9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -530,7 +608,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0">
+    <comment ref="H9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -556,7 +634,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0">
+    <comment ref="I9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -582,7 +660,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J8" authorId="0">
+    <comment ref="J9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -606,7 +684,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0">
+    <comment ref="G10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -632,7 +710,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0">
+    <comment ref="J10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -656,7 +734,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0">
+    <comment ref="G11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -682,7 +760,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J10" authorId="0">
+    <comment ref="J11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -706,7 +784,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0">
+    <comment ref="G12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -732,7 +810,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J11" authorId="0">
+    <comment ref="J12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -756,7 +834,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0">
+    <comment ref="E13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -781,7 +859,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="0">
+    <comment ref="G13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -807,7 +885,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J12" authorId="0">
+    <comment ref="J13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -831,7 +909,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G13" authorId="0">
+    <comment ref="G14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -857,7 +935,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J13" authorId="0">
+    <comment ref="J14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -881,7 +959,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J14" authorId="0">
+    <comment ref="J15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -911,40 +989,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="27">
-  <si>
-    <t>CASO 01</t>
-  </si>
-  <si>
-    <t>CASO 02</t>
-  </si>
-  <si>
-    <t>CASO 03</t>
-  </si>
-  <si>
-    <t>CASO 04</t>
-  </si>
-  <si>
-    <t>CASO 05</t>
-  </si>
-  <si>
-    <t>CASO 06</t>
-  </si>
-  <si>
-    <t>CASO 07</t>
-  </si>
-  <si>
-    <t>CASO 08</t>
-  </si>
-  <si>
-    <t>CASO 09</t>
-  </si>
-  <si>
-    <t>CASO 10</t>
-  </si>
-  <si>
-    <t>CASO 11</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="29">
   <si>
     <t>A</t>
   </si>
@@ -982,16 +1027,55 @@
     <t>I</t>
   </si>
   <si>
-    <t>CASO 12</t>
-  </si>
-  <si>
     <t>Presenta un error en la generacion del archivo de salida, para los casos que encuentra numero M buscado. Luego del "SI" escribe en la linea siguiente la cantidad de ocurrencias y luego la/las posiciones donde comienza M. En los casos en que no hay ocurrencias no presenta fallas, ya que solo debe imprimir "NO".</t>
   </si>
   <si>
     <t>La primera particularidad, a diferencia de los demas ejecutables, es que la aplicación pedia "Presionar una tecla para continuar.." desde la consola, siempre y cuando no quedara colgada. Ademas se presento una anomalia en 2 casos, con M igual a 10 digitos y otro igual a 250, la apliacion quedaba unos segundos iniciada sin responder y luego se cerraba, generando el archivo de Salida vacio. Por lo que presentaria un error de procesamiento, no pudiendo cumplir el requerimiento de longitud de M, tal que 1&lt;=M&lt;=N.</t>
   </si>
   <si>
-    <t>En los casos de prueba 7-8-9-10-11, donde M era "25", detectamos el siguiente patron: la aplicación devolvia todas las posiciones en donde encontraba un "3" y el numero de la posicion terminaba en "3". Luego de imprimir todas estas posiciones imprimia la posicion donde encontraba la ocurrencia del "25", si asi lo existiese.</t>
+    <t>01_UnicoDigitoParaM</t>
+  </si>
+  <si>
+    <t>02_DosDigitosIgualesParaM</t>
+  </si>
+  <si>
+    <t>03_NMIguales</t>
+  </si>
+  <si>
+    <t>04_NMIgualesInvertidos</t>
+  </si>
+  <si>
+    <t>05_NMBinarios</t>
+  </si>
+  <si>
+    <t>06_MCapicua</t>
+  </si>
+  <si>
+    <t>07_FatigaConN20</t>
+  </si>
+  <si>
+    <t>08_FatigaConN50</t>
+  </si>
+  <si>
+    <t>09_FatigaConN100</t>
+  </si>
+  <si>
+    <t>10_FatigaConN250Exito</t>
+  </si>
+  <si>
+    <t>11_FatigaConN250SinExito</t>
+  </si>
+  <si>
+    <t>12_FatigaConNM250</t>
+  </si>
+  <si>
+    <t>00_Enunciado</t>
+  </si>
+  <si>
+    <t>En los casos de prueba 7-8-9-10-11, donde M era "25" y N diferentes longitudes, detectamos el siguiente patron: la aplicación devolvia todas las posiciones en donde encontraba un "3" y el numero de la posicion terminaba en "3". Luego de imprimir todas estas posiciones imprimia la posicion donde encontraba la ocurrencia del "25", si asi lo existiese.</t>
+  </si>
+  <si>
+    <t>OBSERVACION</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1059,8 +1143,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1118,31 +1208,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1151,26 +1221,29 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1473,455 +1546,491 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
       <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+      <c r="A2" s="9"/>
       <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="L2" s="5"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="K4" s="4"/>
       <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="L5" s="5"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="L6" s="5"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="L10" s="5"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="4"/>
+        <v>7</v>
+      </c>
       <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1937,76 +2046,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B10"/>
+  <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="60" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="69.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C2" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="2:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="11"/>
-    </row>
-    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="11"/>
-    </row>
-    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="11"/>
-    </row>
-    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="11"/>
-    </row>
-    <row r="6" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="11"/>
-    </row>
-    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="11"/>
-    </row>
-    <row r="10" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>